<commit_message>
Codigo 1 sin ack con diferente payload
</commit_message>
<xml_diff>
--- a/Pruebas sin ACK.xlsx
+++ b/Pruebas sin ACK.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kYDke\Desktop\NetSoSe\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A37F9532-BC54-4947-A505-8D856E721AE3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85BF4032-A670-4A39-B9C4-C292767F7225}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{83ADD33A-3D7B-44BB-ACDB-DF7CC181FB11}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{83ADD33A-3D7B-44BB-ACDB-DF7CC181FB11}"/>
   </bookViews>
   <sheets>
-    <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
+    <sheet name="Retardos1" sheetId="1" r:id="rId1"/>
+    <sheet name="Retardos2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="10">
   <si>
     <t>t1</t>
   </si>
@@ -43,6 +44,27 @@
   </si>
   <si>
     <t>Promedio</t>
+  </si>
+  <si>
+    <t>Broadcast</t>
+  </si>
+  <si>
+    <t>Unicast</t>
+  </si>
+  <si>
+    <t>Payload 12 bytes</t>
+  </si>
+  <si>
+    <t>Payload 18 bytes</t>
+  </si>
+  <si>
+    <t>Payload 50 bytes</t>
+  </si>
+  <si>
+    <t>Payload 102 bytes</t>
+  </si>
+  <si>
+    <t>Payload 114 bytes</t>
   </si>
 </sst>
 </file>
@@ -86,9 +108,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -104,6 +129,172 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>312420</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>15240</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="3578800" cy="609013"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="CuadroTexto 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{17946C75-7E6C-4F45-833C-853A27AF66CD}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="312420" y="198120"/>
+          <a:ext cx="3578800" cy="609013"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="bg1"/>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="es-EC" sz="1100" b="1"/>
+            <a:t>Código</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="es-EC" sz="1100" b="1" baseline="0"/>
+            <a:t> 1 sin CK</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="es-EC" sz="1100" b="0"/>
+            <a:t>Se</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="es-EC" sz="1100" b="0" baseline="0"/>
+            <a:t> envía una trama desde el coordinador al nodo, </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="es-EC" sz="1100" b="0" baseline="0"/>
+            <a:t>el nodo responde enviando una trama hacia el coordinador</a:t>
+          </a:r>
+          <a:endParaRPr lang="es-EC" sz="1100" b="0"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>53340</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="5212080" cy="609013"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4" name="CuadroTexto 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DDD2D9D9-BCBE-463F-B8AF-CE47A6E49464}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3284220" y="53340"/>
+          <a:ext cx="5212080" cy="609013"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="bg1"/>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="es-EC" sz="1100" b="1"/>
+            <a:t>Código</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="es-EC" sz="1100" b="1" baseline="0"/>
+            <a:t> 1 sin CK</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="es-EC" sz="1100" b="0"/>
+            <a:t>Se</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="es-EC" sz="1100" b="0" baseline="0"/>
+            <a:t> envía una trama desde el coordinador al nodo, el nodo responde enviando una trama hacia el coordinador. Se varia el payload.</a:t>
+          </a:r>
+          <a:endParaRPr lang="es-EC" sz="1100" b="0"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -403,124 +594,36 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F980E90-BBD3-4893-BD89-5054AF332662}">
-  <dimension ref="A1:E13"/>
+  <dimension ref="A6:E20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" s="2"/>
+      <c r="D6" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E6" s="2"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B8" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E1" s="1" t="s">
+      <c r="D8" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E8" s="1" t="s">
         <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2">
-        <v>0</v>
-      </c>
-      <c r="B2">
-        <v>1931</v>
-      </c>
-      <c r="D2">
-        <v>0</v>
-      </c>
-      <c r="E2">
-        <v>2256</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3">
-        <v>0</v>
-      </c>
-      <c r="B3">
-        <v>2902</v>
-      </c>
-      <c r="D3">
-        <v>0</v>
-      </c>
-      <c r="E3">
-        <v>1934</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4">
-        <v>0</v>
-      </c>
-      <c r="B4">
-        <v>3539</v>
-      </c>
-      <c r="D4">
-        <v>0</v>
-      </c>
-      <c r="E4">
-        <v>3209</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5">
-        <v>0</v>
-      </c>
-      <c r="B5">
-        <v>2595</v>
-      </c>
-      <c r="D5">
-        <v>0</v>
-      </c>
-      <c r="E5">
-        <v>3535</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A6">
-        <v>0</v>
-      </c>
-      <c r="B6">
-        <v>1311</v>
-      </c>
-      <c r="D6">
-        <v>0</v>
-      </c>
-      <c r="E6">
-        <v>3536</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A7">
-        <v>0</v>
-      </c>
-      <c r="B7">
-        <v>2261</v>
-      </c>
-      <c r="D7">
-        <v>0</v>
-      </c>
-      <c r="E7">
-        <v>2896</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A8">
-        <v>0</v>
-      </c>
-      <c r="B8">
-        <v>2254</v>
-      </c>
-      <c r="D8">
-        <v>0</v>
-      </c>
-      <c r="E8">
-        <v>3542</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
@@ -528,13 +631,13 @@
         <v>0</v>
       </c>
       <c r="B9">
+        <v>1931</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="E9">
         <v>2256</v>
-      </c>
-      <c r="D9">
-        <v>0</v>
-      </c>
-      <c r="E9">
-        <v>1316</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
@@ -542,13 +645,13 @@
         <v>0</v>
       </c>
       <c r="B10">
-        <v>2896</v>
+        <v>2902</v>
       </c>
       <c r="D10">
         <v>0</v>
       </c>
       <c r="E10">
-        <v>1314</v>
+        <v>1934</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
@@ -556,32 +659,557 @@
         <v>0</v>
       </c>
       <c r="B11">
+        <v>3539</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+      <c r="E11">
+        <v>3209</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>0</v>
+      </c>
+      <c r="B12">
+        <v>2595</v>
+      </c>
+      <c r="D12">
+        <v>0</v>
+      </c>
+      <c r="E12">
+        <v>3535</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>0</v>
+      </c>
+      <c r="B13">
+        <v>1311</v>
+      </c>
+      <c r="D13">
+        <v>0</v>
+      </c>
+      <c r="E13">
+        <v>3536</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>0</v>
+      </c>
+      <c r="B14">
+        <v>2261</v>
+      </c>
+      <c r="D14">
+        <v>0</v>
+      </c>
+      <c r="E14">
+        <v>2896</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>0</v>
+      </c>
+      <c r="B15">
+        <v>2254</v>
+      </c>
+      <c r="D15">
+        <v>0</v>
+      </c>
+      <c r="E15">
+        <v>3542</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>0</v>
+      </c>
+      <c r="B16">
+        <v>2256</v>
+      </c>
+      <c r="D16">
+        <v>0</v>
+      </c>
+      <c r="E16">
+        <v>1316</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>0</v>
+      </c>
+      <c r="B17">
+        <v>2896</v>
+      </c>
+      <c r="D17">
+        <v>0</v>
+      </c>
+      <c r="E17">
+        <v>1314</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <v>0</v>
+      </c>
+      <c r="B18">
         <v>2581</v>
       </c>
+      <c r="D18">
+        <v>0</v>
+      </c>
+      <c r="E18">
+        <v>2898</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A20" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B20">
+        <f>AVERAGE(B9:B18)</f>
+        <v>2452.6</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E20">
+        <f>AVERAGE(E9:E18)</f>
+        <v>2643.6</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="D6:E6"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D14DEFA-C83C-406E-89DA-4177BF284858}">
+  <dimension ref="A5:N18"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G24" sqref="G24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="M5" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="M7" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="N7" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>0</v>
+      </c>
+      <c r="B8">
+        <v>2489</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="E8">
+        <v>2691</v>
+      </c>
+      <c r="G8">
+        <v>0</v>
+      </c>
+      <c r="H8">
+        <v>5091</v>
+      </c>
+      <c r="J8">
+        <v>0</v>
+      </c>
+      <c r="K8">
+        <v>6594</v>
+      </c>
+      <c r="M8">
+        <v>0</v>
+      </c>
+      <c r="N8">
+        <v>6996</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>0</v>
+      </c>
+      <c r="B9">
+        <v>1850</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="E9">
+        <v>1749</v>
+      </c>
+      <c r="G9">
+        <v>0</v>
+      </c>
+      <c r="H9">
+        <v>3174</v>
+      </c>
+      <c r="J9">
+        <v>0</v>
+      </c>
+      <c r="K9">
+        <v>5626</v>
+      </c>
+      <c r="M9">
+        <v>0</v>
+      </c>
+      <c r="N9">
+        <v>7325</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>0</v>
+      </c>
+      <c r="B10">
+        <v>2490</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="E10">
+        <v>2703</v>
+      </c>
+      <c r="G10">
+        <v>0</v>
+      </c>
+      <c r="H10">
+        <v>3494</v>
+      </c>
+      <c r="J10">
+        <v>0</v>
+      </c>
+      <c r="K10">
+        <v>5609</v>
+      </c>
+      <c r="M10">
+        <v>0</v>
+      </c>
+      <c r="N10">
+        <v>5080</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>0</v>
+      </c>
+      <c r="B11">
+        <v>3448</v>
+      </c>
       <c r="D11">
         <v>0</v>
       </c>
       <c r="E11">
-        <v>2898</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A13" s="1" t="s">
+        <v>1749</v>
+      </c>
+      <c r="G11">
+        <v>0</v>
+      </c>
+      <c r="H11">
+        <v>5086</v>
+      </c>
+      <c r="J11">
+        <v>0</v>
+      </c>
+      <c r="K11">
+        <v>4974</v>
+      </c>
+      <c r="M11">
+        <v>0</v>
+      </c>
+      <c r="N11">
+        <v>6034</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>0</v>
+      </c>
+      <c r="B12">
+        <v>2513</v>
+      </c>
+      <c r="D12">
+        <v>0</v>
+      </c>
+      <c r="E12">
+        <v>3343</v>
+      </c>
+      <c r="G12">
+        <v>0</v>
+      </c>
+      <c r="H12">
+        <v>5112</v>
+      </c>
+      <c r="J12">
+        <v>0</v>
+      </c>
+      <c r="K12">
+        <v>6892</v>
+      </c>
+      <c r="M12">
+        <v>0</v>
+      </c>
+      <c r="N12">
+        <v>6669</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>0</v>
+      </c>
+      <c r="B13">
+        <v>3129</v>
+      </c>
+      <c r="D13">
+        <v>0</v>
+      </c>
+      <c r="E13">
+        <v>2392</v>
+      </c>
+      <c r="G13">
+        <v>0</v>
+      </c>
+      <c r="H13">
+        <v>4785</v>
+      </c>
+      <c r="J13">
+        <v>0</v>
+      </c>
+      <c r="K13">
+        <v>5620</v>
+      </c>
+      <c r="M13">
+        <v>0</v>
+      </c>
+      <c r="N13">
+        <v>5080</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>0</v>
+      </c>
+      <c r="B14">
+        <v>3774</v>
+      </c>
+      <c r="D14">
+        <v>0</v>
+      </c>
+      <c r="E14">
+        <v>2691</v>
+      </c>
+      <c r="G14">
+        <v>0</v>
+      </c>
+      <c r="H14">
+        <v>4447</v>
+      </c>
+      <c r="J14">
+        <v>0</v>
+      </c>
+      <c r="K14">
+        <v>5296</v>
+      </c>
+      <c r="M14">
+        <v>0</v>
+      </c>
+      <c r="N14">
+        <v>5710</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>0</v>
+      </c>
+      <c r="B15">
+        <v>1547</v>
+      </c>
+      <c r="D15">
+        <v>0</v>
+      </c>
+      <c r="E15">
+        <v>3347</v>
+      </c>
+      <c r="G15">
+        <v>0</v>
+      </c>
+      <c r="H15">
+        <v>5093</v>
+      </c>
+      <c r="J15">
+        <v>0</v>
+      </c>
+      <c r="K15">
+        <v>5941</v>
+      </c>
+      <c r="M15">
+        <v>0</v>
+      </c>
+      <c r="N15">
+        <v>6041</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>0</v>
+      </c>
+      <c r="B16">
+        <v>2485</v>
+      </c>
+      <c r="D16">
+        <v>0</v>
+      </c>
+      <c r="E16">
+        <v>2706</v>
+      </c>
+      <c r="G16">
+        <v>0</v>
+      </c>
+      <c r="H16">
+        <v>4136</v>
+      </c>
+      <c r="J16">
+        <v>0</v>
+      </c>
+      <c r="K16">
+        <v>5621</v>
+      </c>
+      <c r="M16">
+        <v>0</v>
+      </c>
+      <c r="N16">
+        <v>6346</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>0</v>
+      </c>
+      <c r="B17">
+        <v>2489</v>
+      </c>
+      <c r="D17">
+        <v>0</v>
+      </c>
+      <c r="E17">
+        <v>3981</v>
+      </c>
+      <c r="G17">
+        <v>0</v>
+      </c>
+      <c r="H17">
+        <v>4776</v>
+      </c>
+      <c r="J17">
+        <v>0</v>
+      </c>
+      <c r="K17">
+        <v>6582</v>
+      </c>
+      <c r="M17">
+        <v>0</v>
+      </c>
+      <c r="N17">
+        <v>5086</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A18" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B13">
-        <f>AVERAGE(B2:B11)</f>
-        <v>2452.6</v>
-      </c>
-      <c r="D13" s="1" t="s">
+      <c r="B18">
+        <f>AVERAGE(B8:B17)</f>
+        <v>2621.4</v>
+      </c>
+      <c r="D18" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E13">
-        <f>AVERAGE(E2:E11)</f>
-        <v>2643.6</v>
+      <c r="E18">
+        <f>AVERAGE(E8:E17)</f>
+        <v>2735.2</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="H18">
+        <f>AVERAGE(H8:H17)</f>
+        <v>4519.3999999999996</v>
+      </c>
+      <c r="J18" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="K18">
+        <f>AVERAGE(K8:K17)</f>
+        <v>5875.5</v>
+      </c>
+      <c r="M18" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="N18">
+        <f>AVERAGE(N8:N17)</f>
+        <v>6036.7</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Comprobacion de direccion y payload.Payload Variable
</commit_message>
<xml_diff>
--- a/Pruebas sin ACK.xlsx
+++ b/Pruebas sin ACK.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kYDke\Desktop\NetSoSe\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85BF4032-A670-4A39-B9C4-C292767F7225}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71A8B5F0-F3EC-4BFD-A7FB-1A2F706EF445}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{83ADD33A-3D7B-44BB-ACDB-DF7CC181FB11}"/>
+    <workbookView xWindow="0" yWindow="2616" windowWidth="23040" windowHeight="9744" activeTab="2" xr2:uid="{83ADD33A-3D7B-44BB-ACDB-DF7CC181FB11}"/>
   </bookViews>
   <sheets>
     <sheet name="Retardos1" sheetId="1" r:id="rId1"/>
     <sheet name="Retardos2" sheetId="2" r:id="rId2"/>
+    <sheet name="Retardos3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="11">
   <si>
     <t>t1</t>
   </si>
@@ -65,6 +66,9 @@
   </si>
   <si>
     <t>Payload 114 bytes</t>
+  </si>
+  <si>
+    <t>t3(us)</t>
   </si>
 </sst>
 </file>
@@ -796,8 +800,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D14DEFA-C83C-406E-89DA-4177BF284858}">
   <dimension ref="A5:N18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G24" sqref="G24"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5:N18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1212,4 +1216,614 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1DB411F8-E539-411F-89E9-4C22DC4EF174}">
+  <dimension ref="A5:S18"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="P17" sqref="P17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="M5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q5" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H7" s="1"/>
+      <c r="I7" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="M7" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="N7" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="O7" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q7" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="R7" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="S7" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>0</v>
+      </c>
+      <c r="B8">
+        <v>2471</v>
+      </c>
+      <c r="C8">
+        <v>1673617</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
+      <c r="F8">
+        <v>2359</v>
+      </c>
+      <c r="G8">
+        <v>1656254</v>
+      </c>
+      <c r="I8">
+        <v>0</v>
+      </c>
+      <c r="J8">
+        <v>3445</v>
+      </c>
+      <c r="K8">
+        <v>1652082</v>
+      </c>
+      <c r="M8">
+        <v>0</v>
+      </c>
+      <c r="N8">
+        <v>4899</v>
+      </c>
+      <c r="O8">
+        <v>1641943</v>
+      </c>
+      <c r="Q8">
+        <v>0</v>
+      </c>
+      <c r="R8">
+        <v>2489</v>
+      </c>
+      <c r="S8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>0</v>
+      </c>
+      <c r="B9">
+        <v>3429</v>
+      </c>
+      <c r="C9">
+        <v>1678018</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
+      <c r="F9">
+        <v>1734</v>
+      </c>
+      <c r="G9">
+        <v>1654697</v>
+      </c>
+      <c r="I9">
+        <v>0</v>
+      </c>
+      <c r="J9">
+        <v>4733</v>
+      </c>
+      <c r="K9">
+        <v>1651979</v>
+      </c>
+      <c r="M9">
+        <v>0</v>
+      </c>
+      <c r="N9">
+        <v>5217</v>
+      </c>
+      <c r="O9">
+        <v>1652252</v>
+      </c>
+      <c r="Q9">
+        <v>0</v>
+      </c>
+      <c r="R9">
+        <v>1850</v>
+      </c>
+      <c r="S9">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>0</v>
+      </c>
+      <c r="B10">
+        <v>2793</v>
+      </c>
+      <c r="C10">
+        <v>1675154</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
+      <c r="F10">
+        <v>3001</v>
+      </c>
+      <c r="G10">
+        <v>1654310</v>
+      </c>
+      <c r="I10">
+        <v>0</v>
+      </c>
+      <c r="J10">
+        <v>4731</v>
+      </c>
+      <c r="K10">
+        <v>1664343</v>
+      </c>
+      <c r="M10">
+        <v>0</v>
+      </c>
+      <c r="N10">
+        <v>6811</v>
+      </c>
+      <c r="O10">
+        <v>1652011</v>
+      </c>
+      <c r="Q10">
+        <v>0</v>
+      </c>
+      <c r="R10">
+        <v>2490</v>
+      </c>
+      <c r="S10">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>0</v>
+      </c>
+      <c r="B11">
+        <v>1836</v>
+      </c>
+      <c r="C11">
+        <v>1672268</v>
+      </c>
+      <c r="E11">
+        <v>0</v>
+      </c>
+      <c r="F11">
+        <v>3312</v>
+      </c>
+      <c r="G11">
+        <v>1651881</v>
+      </c>
+      <c r="I11">
+        <v>0</v>
+      </c>
+      <c r="J11">
+        <v>5046</v>
+      </c>
+      <c r="K11">
+        <v>1650478</v>
+      </c>
+      <c r="M11">
+        <v>0</v>
+      </c>
+      <c r="N11">
+        <v>6496</v>
+      </c>
+      <c r="O11">
+        <v>1650900</v>
+      </c>
+      <c r="Q11">
+        <v>0</v>
+      </c>
+      <c r="R11">
+        <v>3448</v>
+      </c>
+      <c r="S11">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>0</v>
+      </c>
+      <c r="B12">
+        <v>2152</v>
+      </c>
+      <c r="C12">
+        <v>1670577</v>
+      </c>
+      <c r="E12">
+        <v>0</v>
+      </c>
+      <c r="F12">
+        <v>1724</v>
+      </c>
+      <c r="G12">
+        <v>1656887</v>
+      </c>
+      <c r="I12">
+        <v>0</v>
+      </c>
+      <c r="J12">
+        <v>4405</v>
+      </c>
+      <c r="K12">
+        <v>1652135</v>
+      </c>
+      <c r="M12">
+        <v>0</v>
+      </c>
+      <c r="N12">
+        <v>6179</v>
+      </c>
+      <c r="O12">
+        <v>1652319</v>
+      </c>
+      <c r="Q12">
+        <v>0</v>
+      </c>
+      <c r="R12">
+        <v>2513</v>
+      </c>
+      <c r="S12">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>0</v>
+      </c>
+      <c r="B13">
+        <v>2478</v>
+      </c>
+      <c r="C13">
+        <v>1671548</v>
+      </c>
+      <c r="E13">
+        <v>0</v>
+      </c>
+      <c r="F13">
+        <v>1743</v>
+      </c>
+      <c r="G13">
+        <v>1661782</v>
+      </c>
+      <c r="I13">
+        <v>0</v>
+      </c>
+      <c r="J13">
+        <v>4400</v>
+      </c>
+      <c r="K13">
+        <v>1653861</v>
+      </c>
+      <c r="M13">
+        <v>0</v>
+      </c>
+      <c r="N13">
+        <v>6816</v>
+      </c>
+      <c r="O13">
+        <v>1648933</v>
+      </c>
+      <c r="Q13">
+        <v>0</v>
+      </c>
+      <c r="R13">
+        <v>3129</v>
+      </c>
+      <c r="S13">
+        <v>1323</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>0</v>
+      </c>
+      <c r="B14">
+        <v>2468</v>
+      </c>
+      <c r="C14">
+        <v>1671292</v>
+      </c>
+      <c r="E14">
+        <v>0</v>
+      </c>
+      <c r="F14">
+        <v>3318</v>
+      </c>
+      <c r="G14">
+        <v>1653395</v>
+      </c>
+      <c r="I14">
+        <v>0</v>
+      </c>
+      <c r="J14">
+        <v>3443</v>
+      </c>
+      <c r="K14">
+        <v>1651521</v>
+      </c>
+      <c r="M14">
+        <v>0</v>
+      </c>
+      <c r="N14">
+        <v>4581</v>
+      </c>
+      <c r="O14">
+        <v>1651365</v>
+      </c>
+      <c r="Q14">
+        <v>0</v>
+      </c>
+      <c r="R14">
+        <v>3774</v>
+      </c>
+      <c r="S14">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>0</v>
+      </c>
+      <c r="B15">
+        <v>3430</v>
+      </c>
+      <c r="C15">
+        <v>1670623</v>
+      </c>
+      <c r="E15">
+        <v>0</v>
+      </c>
+      <c r="F15">
+        <v>2673</v>
+      </c>
+      <c r="G15">
+        <v>1655381</v>
+      </c>
+      <c r="I15">
+        <v>0</v>
+      </c>
+      <c r="J15">
+        <v>4092</v>
+      </c>
+      <c r="K15">
+        <v>1657727</v>
+      </c>
+      <c r="M15">
+        <v>0</v>
+      </c>
+      <c r="N15">
+        <v>6175</v>
+      </c>
+      <c r="O15">
+        <v>1651273</v>
+      </c>
+      <c r="Q15">
+        <v>0</v>
+      </c>
+      <c r="R15">
+        <v>1547</v>
+      </c>
+      <c r="S15">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>0</v>
+      </c>
+      <c r="B16">
+        <v>1530</v>
+      </c>
+      <c r="C16">
+        <v>1664429</v>
+      </c>
+      <c r="E16">
+        <v>0</v>
+      </c>
+      <c r="F16">
+        <v>3959</v>
+      </c>
+      <c r="G16">
+        <v>1652185</v>
+      </c>
+      <c r="I16">
+        <v>0</v>
+      </c>
+      <c r="J16">
+        <v>4084</v>
+      </c>
+      <c r="K16">
+        <v>1652406</v>
+      </c>
+      <c r="M16">
+        <v>0</v>
+      </c>
+      <c r="N16">
+        <v>5859</v>
+      </c>
+      <c r="O16">
+        <v>1650342</v>
+      </c>
+      <c r="Q16">
+        <v>0</v>
+      </c>
+      <c r="R16">
+        <v>2485</v>
+      </c>
+      <c r="S16">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>0</v>
+      </c>
+      <c r="B17">
+        <v>1520</v>
+      </c>
+      <c r="C17">
+        <v>1676304</v>
+      </c>
+      <c r="E17">
+        <v>0</v>
+      </c>
+      <c r="F17">
+        <v>2351</v>
+      </c>
+      <c r="G17">
+        <v>1654923</v>
+      </c>
+      <c r="I17">
+        <v>0</v>
+      </c>
+      <c r="J17">
+        <v>3122</v>
+      </c>
+      <c r="K17">
+        <v>1652254</v>
+      </c>
+      <c r="M17">
+        <v>0</v>
+      </c>
+      <c r="N17">
+        <v>5848</v>
+      </c>
+      <c r="O17">
+        <v>1650682</v>
+      </c>
+      <c r="Q17">
+        <v>0</v>
+      </c>
+      <c r="R17">
+        <v>2489</v>
+      </c>
+      <c r="S17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A18" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B18">
+        <f>AVERAGE(B8:B17)</f>
+        <v>2410.6999999999998</v>
+      </c>
+      <c r="C18">
+        <f>AVERAGE(C8:C17)</f>
+        <v>1672383</v>
+      </c>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F18">
+        <f>AVERAGE(F8:F17)</f>
+        <v>2617.4</v>
+      </c>
+      <c r="G18">
+        <f>AVERAGE(G8:G17)</f>
+        <v>1655169.5</v>
+      </c>
+      <c r="I18" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="J18">
+        <f>AVERAGE(J8:J17)</f>
+        <v>4150.1000000000004</v>
+      </c>
+      <c r="K18">
+        <f>AVERAGE(K8:K17)</f>
+        <v>1653878.6</v>
+      </c>
+      <c r="M18" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="N18">
+        <f>AVERAGE(N8:N17)</f>
+        <v>5888.1</v>
+      </c>
+      <c r="O18">
+        <f>AVERAGE(O8:O17)</f>
+        <v>1650202</v>
+      </c>
+      <c r="Q18" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="R18">
+        <f>AVERAGE(R8:R17)</f>
+        <v>2621.4</v>
+      </c>
+      <c r="S18">
+        <f>AVERAGE(S8:S17)</f>
+        <v>146.69999999999999</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Codigo 2 comentado y codigo 3 creado
</commit_message>
<xml_diff>
--- a/Pruebas sin ACK.xlsx
+++ b/Pruebas sin ACK.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kYDke\Desktop\NetSoSe\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71A8B5F0-F3EC-4BFD-A7FB-1A2F706EF445}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{303B6234-E1A6-4FCC-A604-1AE9C5DD8BBC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2616" windowWidth="23040" windowHeight="9744" activeTab="2" xr2:uid="{83ADD33A-3D7B-44BB-ACDB-DF7CC181FB11}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{83ADD33A-3D7B-44BB-ACDB-DF7CC181FB11}"/>
   </bookViews>
   <sheets>
     <sheet name="Retardos1" sheetId="1" r:id="rId1"/>
@@ -293,6 +293,140 @@
             <a:t> envía una trama desde el coordinador al nodo, el nodo responde enviando una trama hacia el coordinador. Se varia el payload.</a:t>
           </a:r>
           <a:endParaRPr lang="es-EC" sz="1100" b="0"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>30480</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="7354834" cy="670560"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="CuadroTexto 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{90F1496C-0493-4C9B-9FFD-05F35735FAFF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3284220" y="30480"/>
+          <a:ext cx="7354834" cy="670560"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="bg1"/>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:noAutofit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="es-EC" sz="1100" b="1">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Código</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="es-EC" sz="1100" b="1" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t> 1 sin CK</a:t>
+          </a:r>
+          <a:endParaRPr lang="es-EC">
+            <a:effectLst/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="es-EC" sz="1100" b="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Se</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="es-EC" sz="1100" b="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t> envía una trama desde el coordinador al nodo, el nodo responde enviando una trama hacia el coordinador. El coordinador</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="es-EC" sz="1100" b="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>entonces compara el payload y la direccion origen para proceder a responder con otra trama.</a:t>
+          </a:r>
+          <a:endParaRPr lang="es-EC">
+            <a:effectLst/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="es-EC" sz="1100"/>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
@@ -1222,8 +1356,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1DB411F8-E539-411F-89E9-4C22DC4EF174}">
   <dimension ref="A5:S18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="P17" sqref="P17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="S18" sqref="S18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1336,10 +1470,10 @@
         <v>0</v>
       </c>
       <c r="R8">
-        <v>2489</v>
+        <v>5941</v>
       </c>
       <c r="S8">
-        <v>1</v>
+        <v>1694510</v>
       </c>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.3">
@@ -1383,10 +1517,10 @@
         <v>0</v>
       </c>
       <c r="R9">
-        <v>1850</v>
+        <v>5611</v>
       </c>
       <c r="S9">
-        <v>3</v>
+        <v>1685108</v>
       </c>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.3">
@@ -1430,10 +1564,10 @@
         <v>0</v>
       </c>
       <c r="R10">
-        <v>2490</v>
+        <v>6891</v>
       </c>
       <c r="S10">
-        <v>4</v>
+        <v>1696078</v>
       </c>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.3">
@@ -1477,10 +1611,10 @@
         <v>0</v>
       </c>
       <c r="R11">
-        <v>3448</v>
+        <v>7662</v>
       </c>
       <c r="S11">
-        <v>123</v>
+        <v>1693462</v>
       </c>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.3">
@@ -1524,10 +1658,10 @@
         <v>0</v>
       </c>
       <c r="R12">
-        <v>2513</v>
+        <v>6258</v>
       </c>
       <c r="S12">
-        <v>3</v>
+        <v>1697605</v>
       </c>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.3">
@@ -1571,10 +1705,10 @@
         <v>0</v>
       </c>
       <c r="R13">
-        <v>3129</v>
+        <v>6897</v>
       </c>
       <c r="S13">
-        <v>1323</v>
+        <v>1692796</v>
       </c>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.3">
@@ -1618,10 +1752,10 @@
         <v>0</v>
       </c>
       <c r="R14">
-        <v>3774</v>
+        <v>5295</v>
       </c>
       <c r="S14">
-        <v>4</v>
+        <v>1693505</v>
       </c>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.3">
@@ -1665,10 +1799,10 @@
         <v>0</v>
       </c>
       <c r="R15">
-        <v>1547</v>
+        <v>6584</v>
       </c>
       <c r="S15">
-        <v>3</v>
+        <v>1695937</v>
       </c>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.3">
@@ -1712,10 +1846,10 @@
         <v>0</v>
       </c>
       <c r="R16">
-        <v>2485</v>
+        <v>6579</v>
       </c>
       <c r="S16">
-        <v>2</v>
+        <v>1692608</v>
       </c>
     </row>
     <row r="17" spans="1:19" x14ac:dyDescent="0.3">
@@ -1759,10 +1893,10 @@
         <v>0</v>
       </c>
       <c r="R17">
-        <v>2489</v>
+        <v>5622</v>
       </c>
       <c r="S17">
-        <v>1</v>
+        <v>1696778</v>
       </c>
     </row>
     <row r="18" spans="1:19" x14ac:dyDescent="0.3">
@@ -1816,14 +1950,15 @@
       </c>
       <c r="R18">
         <f>AVERAGE(R8:R17)</f>
-        <v>2621.4</v>
+        <v>6334</v>
       </c>
       <c r="S18">
         <f>AVERAGE(S8:S17)</f>
-        <v>146.69999999999999</v>
+        <v>1693838.7</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Codigo 3 Implementado y Codigo 2 arreglado
</commit_message>
<xml_diff>
--- a/Pruebas sin ACK.xlsx
+++ b/Pruebas sin ACK.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kYDke\Desktop\NetSoSe\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{303B6234-E1A6-4FCC-A604-1AE9C5DD8BBC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A172EBB-BE8A-470B-A60A-47D19631860F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{83ADD33A-3D7B-44BB-ACDB-DF7CC181FB11}"/>
+    <workbookView xWindow="6936" yWindow="768" windowWidth="23040" windowHeight="9744" activeTab="2" xr2:uid="{83ADD33A-3D7B-44BB-ACDB-DF7CC181FB11}"/>
   </bookViews>
   <sheets>
     <sheet name="Retardos1" sheetId="1" r:id="rId1"/>
@@ -310,7 +310,7 @@
       <xdr:row>0</xdr:row>
       <xdr:rowOff>30480</xdr:rowOff>
     </xdr:from>
-    <xdr:ext cx="7354834" cy="670560"/>
+    <xdr:ext cx="7719060" cy="670560"/>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
         <xdr:cNvPr id="2" name="CuadroTexto 1">
@@ -325,7 +325,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3284220" y="30480"/>
-          <a:ext cx="7354834" cy="670560"/>
+          <a:ext cx="7719060" cy="670560"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -376,7 +376,7 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t> 1 sin CK</a:t>
+            <a:t> 2 sin CK</a:t>
           </a:r>
           <a:endParaRPr lang="es-EC">
             <a:effectLst/>
@@ -405,7 +405,7 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t> envía una trama desde el coordinador al nodo, el nodo responde enviando una trama hacia el coordinador. El coordinador</a:t>
+            <a:t> envía una trama desde el coordinador al nodo, el nodo responde enviando la misma trama(payload) recibida hacia el coordinador. </a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -419,7 +419,7 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>entonces compara el payload y la direccion origen para proceder a responder con otra trama.</a:t>
+            <a:t>El coordinador entonces compara el payload y la direccion origen con la trama enviada para proceder a responder con otra trama.</a:t>
           </a:r>
           <a:endParaRPr lang="es-EC">
             <a:effectLst/>
@@ -1356,8 +1356,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1DB411F8-E539-411F-89E9-4C22DC4EF174}">
   <dimension ref="A5:S18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S18" sqref="S18"/>
+    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
+      <selection activeCell="O20" sqref="O20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1434,46 +1434,46 @@
         <v>0</v>
       </c>
       <c r="B8">
-        <v>2471</v>
+        <v>2475</v>
       </c>
       <c r="C8">
-        <v>1673617</v>
+        <v>18521</v>
       </c>
       <c r="E8">
         <v>0</v>
       </c>
       <c r="F8">
-        <v>2359</v>
+        <v>2039</v>
       </c>
       <c r="G8">
-        <v>1656254</v>
+        <v>18889</v>
       </c>
       <c r="I8">
         <v>0</v>
       </c>
       <c r="J8">
-        <v>3445</v>
+        <v>4079</v>
       </c>
       <c r="K8">
-        <v>1652082</v>
+        <v>19351</v>
       </c>
       <c r="M8">
         <v>0</v>
       </c>
       <c r="N8">
-        <v>4899</v>
+        <v>4605</v>
       </c>
       <c r="O8">
-        <v>1641943</v>
+        <v>18952</v>
       </c>
       <c r="Q8">
         <v>0</v>
       </c>
       <c r="R8">
-        <v>5941</v>
+        <v>5298</v>
       </c>
       <c r="S8">
-        <v>1694510</v>
+        <v>19611</v>
       </c>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.3">
@@ -1481,46 +1481,46 @@
         <v>0</v>
       </c>
       <c r="B9">
-        <v>3429</v>
+        <v>3129</v>
       </c>
       <c r="C9">
-        <v>1678018</v>
+        <v>17244</v>
       </c>
       <c r="E9">
         <v>0</v>
       </c>
       <c r="F9">
-        <v>1734</v>
+        <v>3971</v>
       </c>
       <c r="G9">
-        <v>1654697</v>
+        <v>18871</v>
       </c>
       <c r="I9">
         <v>0</v>
       </c>
       <c r="J9">
-        <v>4733</v>
+        <v>3450</v>
       </c>
       <c r="K9">
-        <v>1651979</v>
+        <v>15516</v>
       </c>
       <c r="M9">
         <v>0</v>
       </c>
       <c r="N9">
-        <v>5217</v>
+        <v>5534</v>
       </c>
       <c r="O9">
-        <v>1652252</v>
+        <v>18261</v>
       </c>
       <c r="Q9">
         <v>0</v>
       </c>
       <c r="R9">
-        <v>5611</v>
+        <v>6895</v>
       </c>
       <c r="S9">
-        <v>1685108</v>
+        <v>16743</v>
       </c>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.3">
@@ -1528,46 +1528,46 @@
         <v>0</v>
       </c>
       <c r="B10">
-        <v>2793</v>
+        <v>2481</v>
       </c>
       <c r="C10">
-        <v>1675154</v>
+        <v>16603</v>
       </c>
       <c r="E10">
         <v>0</v>
       </c>
       <c r="F10">
-        <v>3001</v>
+        <v>3644</v>
       </c>
       <c r="G10">
-        <v>1654310</v>
+        <v>16230</v>
       </c>
       <c r="I10">
         <v>0</v>
       </c>
       <c r="J10">
-        <v>4731</v>
+        <v>4728</v>
       </c>
       <c r="K10">
-        <v>1664343</v>
+        <v>14089</v>
       </c>
       <c r="M10">
         <v>0</v>
       </c>
       <c r="N10">
-        <v>6811</v>
+        <v>5857</v>
       </c>
       <c r="O10">
-        <v>1652011</v>
+        <v>19273</v>
       </c>
       <c r="Q10">
         <v>0</v>
       </c>
       <c r="R10">
-        <v>6891</v>
+        <v>5620</v>
       </c>
       <c r="S10">
-        <v>1696078</v>
+        <v>17392</v>
       </c>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.3">
@@ -1575,46 +1575,46 @@
         <v>0</v>
       </c>
       <c r="B11">
-        <v>1836</v>
+        <v>1532</v>
       </c>
       <c r="C11">
-        <v>1672268</v>
+        <v>18201</v>
       </c>
       <c r="E11">
         <v>0</v>
       </c>
       <c r="F11">
-        <v>3312</v>
+        <v>2368</v>
       </c>
       <c r="G11">
-        <v>1651881</v>
+        <v>17604</v>
       </c>
       <c r="I11">
         <v>0</v>
       </c>
       <c r="J11">
-        <v>5046</v>
+        <v>3126</v>
       </c>
       <c r="K11">
-        <v>1650478</v>
+        <v>16797</v>
       </c>
       <c r="M11">
         <v>0</v>
       </c>
       <c r="N11">
-        <v>6496</v>
+        <v>5858</v>
       </c>
       <c r="O11">
-        <v>1650900</v>
+        <v>18954</v>
       </c>
       <c r="Q11">
         <v>0</v>
       </c>
       <c r="R11">
-        <v>7662</v>
+        <v>4998</v>
       </c>
       <c r="S11">
-        <v>1693462</v>
+        <v>18670</v>
       </c>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.3">
@@ -1622,46 +1622,46 @@
         <v>0</v>
       </c>
       <c r="B12">
-        <v>2152</v>
+        <v>3755</v>
       </c>
       <c r="C12">
-        <v>1670577</v>
+        <v>19474</v>
       </c>
       <c r="E12">
         <v>0</v>
       </c>
       <c r="F12">
-        <v>1724</v>
+        <v>2043</v>
       </c>
       <c r="G12">
-        <v>1656887</v>
+        <v>17284</v>
       </c>
       <c r="I12">
         <v>0</v>
       </c>
       <c r="J12">
-        <v>4405</v>
+        <v>3440</v>
       </c>
       <c r="K12">
-        <v>1652135</v>
+        <v>17424</v>
       </c>
       <c r="M12">
         <v>0</v>
       </c>
       <c r="N12">
-        <v>6179</v>
+        <v>6818</v>
       </c>
       <c r="O12">
-        <v>1652319</v>
+        <v>17994</v>
       </c>
       <c r="Q12">
         <v>0</v>
       </c>
       <c r="R12">
-        <v>6258</v>
+        <v>6581</v>
       </c>
       <c r="S12">
-        <v>1697605</v>
+        <v>18211</v>
       </c>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.3">
@@ -1669,46 +1669,46 @@
         <v>0</v>
       </c>
       <c r="B13">
-        <v>2478</v>
+        <v>3123</v>
       </c>
       <c r="C13">
-        <v>1671548</v>
+        <v>17246</v>
       </c>
       <c r="E13">
         <v>0</v>
       </c>
       <c r="F13">
-        <v>1743</v>
+        <v>3640</v>
       </c>
       <c r="G13">
-        <v>1661782</v>
+        <v>17367</v>
       </c>
       <c r="I13">
         <v>0</v>
       </c>
       <c r="J13">
-        <v>4400</v>
+        <v>5040</v>
       </c>
       <c r="K13">
-        <v>1653861</v>
+        <v>18049</v>
       </c>
       <c r="M13">
         <v>0</v>
       </c>
       <c r="N13">
-        <v>6816</v>
+        <v>6806</v>
       </c>
       <c r="O13">
-        <v>1648933</v>
+        <v>17997</v>
       </c>
       <c r="Q13">
         <v>0</v>
       </c>
       <c r="R13">
-        <v>6897</v>
+        <v>5612</v>
       </c>
       <c r="S13">
-        <v>1692796</v>
+        <v>17715</v>
       </c>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.3">
@@ -1716,46 +1716,46 @@
         <v>0</v>
       </c>
       <c r="B14">
-        <v>2468</v>
+        <v>2806</v>
       </c>
       <c r="C14">
-        <v>1671292</v>
+        <v>17565</v>
       </c>
       <c r="E14">
         <v>0</v>
       </c>
       <c r="F14">
-        <v>3318</v>
+        <v>3970</v>
       </c>
       <c r="G14">
-        <v>1653395</v>
+        <v>18685</v>
       </c>
       <c r="I14">
         <v>0</v>
       </c>
       <c r="J14">
-        <v>3443</v>
+        <v>2812</v>
       </c>
       <c r="K14">
-        <v>1651521</v>
+        <v>18062</v>
       </c>
       <c r="M14">
         <v>0</v>
       </c>
       <c r="N14">
-        <v>4581</v>
+        <v>4580</v>
       </c>
       <c r="O14">
-        <v>1651365</v>
+        <v>18317</v>
       </c>
       <c r="Q14">
         <v>0</v>
       </c>
       <c r="R14">
-        <v>5295</v>
+        <v>7217</v>
       </c>
       <c r="S14">
-        <v>1693505</v>
+        <v>21681</v>
       </c>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.3">
@@ -1763,46 +1763,46 @@
         <v>0</v>
       </c>
       <c r="B15">
-        <v>3430</v>
+        <v>2483</v>
       </c>
       <c r="C15">
-        <v>1670623</v>
+        <v>16925</v>
       </c>
       <c r="E15">
         <v>0</v>
       </c>
       <c r="F15">
-        <v>2673</v>
+        <v>1739</v>
       </c>
       <c r="G15">
-        <v>1655381</v>
+        <v>14231</v>
       </c>
       <c r="I15">
         <v>0</v>
       </c>
       <c r="J15">
-        <v>4092</v>
+        <v>2821</v>
       </c>
       <c r="K15">
-        <v>1657727</v>
+        <v>17422</v>
       </c>
       <c r="M15">
         <v>0</v>
       </c>
       <c r="N15">
-        <v>6175</v>
+        <v>4608</v>
       </c>
       <c r="O15">
-        <v>1651273</v>
+        <v>17677</v>
       </c>
       <c r="Q15">
         <v>0</v>
       </c>
       <c r="R15">
-        <v>6584</v>
+        <v>7229</v>
       </c>
       <c r="S15">
-        <v>1695937</v>
+        <v>18660</v>
       </c>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.3">
@@ -1810,46 +1810,46 @@
         <v>0</v>
       </c>
       <c r="B16">
-        <v>1530</v>
+        <v>1531</v>
       </c>
       <c r="C16">
-        <v>1664429</v>
+        <v>15644</v>
       </c>
       <c r="E16">
         <v>0</v>
       </c>
       <c r="F16">
-        <v>3959</v>
+        <v>3348</v>
       </c>
       <c r="G16">
-        <v>1652185</v>
+        <v>17286</v>
       </c>
       <c r="I16">
         <v>0</v>
       </c>
       <c r="J16">
-        <v>4084</v>
+        <v>2818</v>
       </c>
       <c r="K16">
-        <v>1652406</v>
+        <v>18048</v>
       </c>
       <c r="M16">
         <v>0</v>
       </c>
       <c r="N16">
-        <v>5859</v>
+        <v>4888</v>
       </c>
       <c r="O16">
-        <v>1650342</v>
+        <v>20221</v>
       </c>
       <c r="Q16">
         <v>0</v>
       </c>
       <c r="R16">
-        <v>6579</v>
+        <v>6263</v>
       </c>
       <c r="S16">
-        <v>1692608</v>
+        <v>22610</v>
       </c>
     </row>
     <row r="17" spans="1:19" x14ac:dyDescent="0.3">
@@ -1857,46 +1857,46 @@
         <v>0</v>
       </c>
       <c r="B17">
-        <v>1520</v>
+        <v>2165</v>
       </c>
       <c r="C17">
-        <v>1676304</v>
+        <v>14404</v>
       </c>
       <c r="E17">
         <v>0</v>
       </c>
       <c r="F17">
-        <v>2351</v>
+        <v>2693</v>
       </c>
       <c r="G17">
-        <v>1654923</v>
+        <v>14271</v>
       </c>
       <c r="I17">
         <v>0</v>
       </c>
       <c r="J17">
-        <v>3122</v>
+        <v>3776</v>
       </c>
       <c r="K17">
-        <v>1652254</v>
+        <v>18386</v>
       </c>
       <c r="M17">
         <v>0</v>
       </c>
       <c r="N17">
-        <v>5848</v>
+        <v>5222</v>
       </c>
       <c r="O17">
-        <v>1650682</v>
+        <v>18302</v>
       </c>
       <c r="Q17">
         <v>0</v>
       </c>
       <c r="R17">
-        <v>5622</v>
+        <v>6910</v>
       </c>
       <c r="S17">
-        <v>1696778</v>
+        <v>16754</v>
       </c>
     </row>
     <row r="18" spans="1:19" x14ac:dyDescent="0.3">
@@ -1905,11 +1905,11 @@
       </c>
       <c r="B18">
         <f>AVERAGE(B8:B17)</f>
-        <v>2410.6999999999998</v>
+        <v>2548</v>
       </c>
       <c r="C18">
         <f>AVERAGE(C8:C17)</f>
-        <v>1672383</v>
+        <v>17182.7</v>
       </c>
       <c r="D18" s="1"/>
       <c r="E18" s="1" t="s">
@@ -1917,44 +1917,44 @@
       </c>
       <c r="F18">
         <f>AVERAGE(F8:F17)</f>
-        <v>2617.4</v>
+        <v>2945.5</v>
       </c>
       <c r="G18">
         <f>AVERAGE(G8:G17)</f>
-        <v>1655169.5</v>
+        <v>17071.8</v>
       </c>
       <c r="I18" s="1" t="s">
         <v>2</v>
       </c>
       <c r="J18">
         <f>AVERAGE(J8:J17)</f>
-        <v>4150.1000000000004</v>
+        <v>3609</v>
       </c>
       <c r="K18">
         <f>AVERAGE(K8:K17)</f>
-        <v>1653878.6</v>
+        <v>17314.400000000001</v>
       </c>
       <c r="M18" s="1" t="s">
         <v>2</v>
       </c>
       <c r="N18">
         <f>AVERAGE(N8:N17)</f>
-        <v>5888.1</v>
+        <v>5477.6</v>
       </c>
       <c r="O18">
         <f>AVERAGE(O8:O17)</f>
-        <v>1650202</v>
+        <v>18594.8</v>
       </c>
       <c r="Q18" s="1" t="s">
         <v>2</v>
       </c>
       <c r="R18">
         <f>AVERAGE(R8:R17)</f>
-        <v>6334</v>
+        <v>6262.3</v>
       </c>
       <c r="S18">
         <f>AVERAGE(S8:S17)</f>
-        <v>1693838.7</v>
+        <v>18804.7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Ultimas pruebas realizadas con IACK. Modificacion codigo IACK2
</commit_message>
<xml_diff>
--- a/Pruebas sin ACK.xlsx
+++ b/Pruebas sin ACK.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kYDke\Desktop\NetSoSe\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A172EBB-BE8A-470B-A60A-47D19631860F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE5DAA7C-DE68-4493-A228-57B03FA8D67C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6936" yWindow="768" windowWidth="23040" windowHeight="9744" activeTab="2" xr2:uid="{83ADD33A-3D7B-44BB-ACDB-DF7CC181FB11}"/>
+    <workbookView xWindow="6924" yWindow="2376" windowWidth="23040" windowHeight="9744" firstSheet="1" activeTab="3" xr2:uid="{83ADD33A-3D7B-44BB-ACDB-DF7CC181FB11}"/>
   </bookViews>
   <sheets>
     <sheet name="Retardos1" sheetId="1" r:id="rId1"/>
     <sheet name="Retardos2" sheetId="2" r:id="rId2"/>
     <sheet name="Retardos3" sheetId="3" r:id="rId3"/>
+    <sheet name="Retardos4" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="14">
   <si>
     <t>t1</t>
   </si>
@@ -69,6 +70,15 @@
   </si>
   <si>
     <t>t3(us)</t>
+  </si>
+  <si>
+    <t>Payload 12 bytes delay 10ms sin procesamiento</t>
+  </si>
+  <si>
+    <t>Payload 12 bytes delay 4ms con procesamiento</t>
+  </si>
+  <si>
+    <t>Payload 12 bytes delay 4ms sin procesamiento</t>
   </si>
 </sst>
 </file>
@@ -1356,8 +1366,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1DB411F8-E539-411F-89E9-4C22DC4EF174}">
   <dimension ref="A5:S18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
-      <selection activeCell="O20" sqref="O20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5:C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1961,4 +1971,384 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40FF73D7-868E-4A27-9B48-A85C41C405F3}">
+  <dimension ref="A5:K18"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="D2" workbookViewId="0">
+      <selection activeCell="I18" sqref="I18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>0</v>
+      </c>
+      <c r="B8">
+        <v>2787</v>
+      </c>
+      <c r="C8">
+        <v>16083</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
+      <c r="F8">
+        <v>2796</v>
+      </c>
+      <c r="G8">
+        <v>6092</v>
+      </c>
+      <c r="I8">
+        <v>0</v>
+      </c>
+      <c r="J8">
+        <v>3425</v>
+      </c>
+      <c r="K8">
+        <v>4913</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>0</v>
+      </c>
+      <c r="B9">
+        <v>3750</v>
+      </c>
+      <c r="C9">
+        <v>16722</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
+      <c r="F9">
+        <v>1835</v>
+      </c>
+      <c r="G9">
+        <v>8014</v>
+      </c>
+      <c r="I9">
+        <v>0</v>
+      </c>
+      <c r="J9">
+        <v>2478</v>
+      </c>
+      <c r="K9">
+        <v>7788</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>0</v>
+      </c>
+      <c r="B10">
+        <v>1525</v>
+      </c>
+      <c r="C10">
+        <v>16085</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
+      <c r="F10">
+        <v>3748</v>
+      </c>
+      <c r="G10">
+        <v>7373</v>
+      </c>
+      <c r="I10">
+        <v>0</v>
+      </c>
+      <c r="J10">
+        <v>2466</v>
+      </c>
+      <c r="K10">
+        <v>6189</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>0</v>
+      </c>
+      <c r="B11">
+        <v>2151</v>
+      </c>
+      <c r="C11">
+        <v>18324</v>
+      </c>
+      <c r="E11">
+        <v>0</v>
+      </c>
+      <c r="F11">
+        <v>3122</v>
+      </c>
+      <c r="G11">
+        <v>6730</v>
+      </c>
+      <c r="I11">
+        <v>0</v>
+      </c>
+      <c r="J11">
+        <v>1524</v>
+      </c>
+      <c r="K11">
+        <v>6508</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>0</v>
+      </c>
+      <c r="B12">
+        <v>2796</v>
+      </c>
+      <c r="C12">
+        <v>17686</v>
+      </c>
+      <c r="E12">
+        <v>0</v>
+      </c>
+      <c r="F12">
+        <v>3436</v>
+      </c>
+      <c r="G12">
+        <v>7691</v>
+      </c>
+      <c r="I12">
+        <v>0</v>
+      </c>
+      <c r="J12">
+        <v>2153</v>
+      </c>
+      <c r="K12">
+        <v>7780</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>0</v>
+      </c>
+      <c r="B13">
+        <v>2153</v>
+      </c>
+      <c r="C13">
+        <v>17363</v>
+      </c>
+      <c r="E13">
+        <v>0</v>
+      </c>
+      <c r="F13">
+        <v>2146</v>
+      </c>
+      <c r="G13">
+        <v>5779</v>
+      </c>
+      <c r="I13">
+        <v>0</v>
+      </c>
+      <c r="J13">
+        <v>1518</v>
+      </c>
+      <c r="K13">
+        <v>5556</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>0</v>
+      </c>
+      <c r="B14">
+        <v>1520</v>
+      </c>
+      <c r="C14">
+        <v>16087</v>
+      </c>
+      <c r="E14">
+        <v>0</v>
+      </c>
+      <c r="F14">
+        <v>3748</v>
+      </c>
+      <c r="G14">
+        <v>7375</v>
+      </c>
+      <c r="I14">
+        <v>0</v>
+      </c>
+      <c r="J14">
+        <v>1830</v>
+      </c>
+      <c r="K14">
+        <v>5876</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>0</v>
+      </c>
+      <c r="B15">
+        <v>3745</v>
+      </c>
+      <c r="C15">
+        <v>16080</v>
+      </c>
+      <c r="E15">
+        <v>0</v>
+      </c>
+      <c r="F15">
+        <v>2476</v>
+      </c>
+      <c r="G15">
+        <v>5451</v>
+      </c>
+      <c r="I15">
+        <v>0</v>
+      </c>
+      <c r="J15">
+        <v>1514</v>
+      </c>
+      <c r="K15">
+        <v>6190</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>0</v>
+      </c>
+      <c r="B16">
+        <v>2167</v>
+      </c>
+      <c r="C16">
+        <v>16091</v>
+      </c>
+      <c r="E16">
+        <v>0</v>
+      </c>
+      <c r="F16">
+        <v>2467</v>
+      </c>
+      <c r="G16">
+        <v>6730</v>
+      </c>
+      <c r="I16">
+        <v>0</v>
+      </c>
+      <c r="J16">
+        <v>3434</v>
+      </c>
+      <c r="K16">
+        <v>6189</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>0</v>
+      </c>
+      <c r="B17">
+        <v>3114</v>
+      </c>
+      <c r="C17">
+        <v>16399</v>
+      </c>
+      <c r="E17">
+        <v>0</v>
+      </c>
+      <c r="F17">
+        <v>1514</v>
+      </c>
+      <c r="G17">
+        <v>5460</v>
+      </c>
+      <c r="I17">
+        <v>0</v>
+      </c>
+      <c r="J17">
+        <v>1510</v>
+      </c>
+      <c r="K17">
+        <v>6499</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A18" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B18">
+        <f>AVERAGE(B8:B17)</f>
+        <v>2570.8000000000002</v>
+      </c>
+      <c r="C18">
+        <f>AVERAGE(C8:C17)</f>
+        <v>16692</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F18">
+        <f>AVERAGE(F8:F17)</f>
+        <v>2728.8</v>
+      </c>
+      <c r="G18">
+        <f>AVERAGE(G8:G17)</f>
+        <v>6669.5</v>
+      </c>
+      <c r="I18" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="J18">
+        <f>AVERAGE(J8:J17)</f>
+        <v>2185.1999999999998</v>
+      </c>
+      <c r="K18">
+        <f>AVERAGE(K8:K17)</f>
+        <v>6348.8</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>